<commit_message>
Updates in DDLs after discussion, phone no and zip
</commit_message>
<xml_diff>
--- a/BLOOD_Bank_MetaData.xlsx
+++ b/BLOOD_Bank_MetaData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22729"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF072C7C-6278-444E-87A5-603349BC9BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{432C1BA2-14DC-4A78-9C94-D12879793C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -764,10 +764,10 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -917,10 +917,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D23">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1095,6 +1095,9 @@
       <c r="C35" t="s">
         <v>9</v>
       </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
       <c r="E35" t="s">
         <v>15</v>
       </c>
@@ -1293,6 +1296,9 @@
       <c r="C49" t="s">
         <v>9</v>
       </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
@@ -1458,10 +1464,10 @@
         <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D62">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E62" t="s">
         <v>10</v>
@@ -1495,10 +1501,10 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D65">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E65" t="s">
         <v>10</v>
@@ -1532,10 +1538,10 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D68">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Update in queries and meatadat excel as discused in meeting
</commit_message>
<xml_diff>
--- a/BLOOD_Bank_MetaData.xlsx
+++ b/BLOOD_Bank_MetaData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22729"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{432C1BA2-14DC-4A78-9C94-D12879793C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C43AA34-1C13-4750-A54F-B14E051812F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="70">
   <si>
     <t>Entity</t>
   </si>
@@ -72,27 +72,30 @@
     <t>VARCHAR</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Bbank_id</t>
+  </si>
+  <si>
+    <t>BLOOD_BANK</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Bbank_id</t>
-  </si>
-  <si>
-    <t>BLOOD_BANK</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Phone_no</t>
   </si>
   <si>
+    <t>BIGINT</t>
+  </si>
+  <si>
     <t>BLOOD_DONATION_EVENT</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
+    <t>Change to data time</t>
+  </si>
+  <si>
     <t>Venue</t>
   </si>
   <si>
@@ -129,6 +135,9 @@
     <t>Btype_Limits</t>
   </si>
   <si>
+    <t>Default 100</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -180,12 +189,18 @@
     <t>BOOLEAN</t>
   </si>
   <si>
+    <t>Default : unpaid</t>
+  </si>
+  <si>
     <t>True for Paid, False for unpaid</t>
   </si>
   <si>
     <t>Notification_Subscription</t>
   </si>
   <si>
+    <t>Default : False</t>
+  </si>
+  <si>
     <t>Notification_Type</t>
   </si>
   <si>
@@ -211,6 +226,9 @@
   </si>
   <si>
     <t>EMERGENCY_CONTACT_EMAIL</t>
+  </si>
+  <si>
+    <t>BIFGINT</t>
   </si>
   <si>
     <t>DBA_LOGIN_CREDENTIALS</t>
@@ -240,12 +258,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -260,10 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,14 +605,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -651,7 +676,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -659,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -676,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -693,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -704,10 +729,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -724,7 +749,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -736,35 +761,35 @@
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -775,10 +800,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -795,7 +820,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -804,35 +829,38 @@
         <v>14</v>
       </c>
       <c r="D14">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -846,7 +874,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -855,12 +883,12 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -877,10 +905,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -894,10 +922,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -911,13 +939,13 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -931,10 +959,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
         <v>31</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -948,10 +976,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -968,44 +996,44 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -1022,27 +1050,27 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1053,10 +1081,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
@@ -1065,15 +1093,15 @@
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
@@ -1082,15 +1110,15 @@
         <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -1099,15 +1127,15 @@
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>9</v>
@@ -1124,10 +1152,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
@@ -1136,66 +1164,66 @@
         <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1203,10 +1231,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1223,7 +1251,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
@@ -1240,13 +1268,13 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1254,10 +1282,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -1266,15 +1294,15 @@
         <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -1283,15 +1311,15 @@
         <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1300,63 +1328,63 @@
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="F50" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -1365,15 +1393,15 @@
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
@@ -1387,10 +1415,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -1407,10 +1435,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
@@ -1424,10 +1452,10 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -1441,10 +1469,10 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
@@ -1458,7 +1486,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>21</v>
@@ -1478,10 +1506,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -1495,7 +1523,7 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>21</v>
@@ -1515,7 +1543,7 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>13</v>
@@ -1527,18 +1555,18 @@
         <v>25</v>
       </c>
       <c r="E66" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="D68">
         <v>10</v>
@@ -1552,10 +1580,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
@@ -1569,10 +1597,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C70" t="s">
         <v>14</v>
@@ -1589,10 +1617,10 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -1609,10 +1637,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" t="s">
         <v>62</v>
-      </c>
-      <c r="B73" t="s">
-        <v>57</v>
       </c>
       <c r="C73" t="s">
         <v>14</v>
@@ -1626,10 +1654,10 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C74" t="s">
         <v>14</v>

</xml_diff>